<commit_message>
Nhat Linh : update final flow for report function admin
</commit_message>
<xml_diff>
--- a/DuLieuThongKe/ThongKeDoanhThuCacNgayTrongThang8-2023.xlsx
+++ b/DuLieuThongKe/ThongKeDoanhThuCacNgayTrongThang8-2023.xlsx
@@ -223,7 +223,7 @@
     <col min="6" max="6" width="19.3671875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="18.11328125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="21.91796875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.62890625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.3203125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -2296,22 +2296,22 @@
         <v>13</v>
       </c>
       <c r="E70" t="n" s="0">
-        <v>997640.0</v>
+        <v>1351990.0</v>
       </c>
       <c r="F70" t="n" s="0">
-        <v>0.0</v>
+        <v>1065000.0</v>
       </c>
       <c r="G70" t="n" s="0">
-        <v>897676.4705135226</v>
+        <v>151414.29498244822</v>
       </c>
       <c r="H70" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="I70" t="n" s="0">
-        <v>99764.00148659945</v>
+        <v>135199.0020146221</v>
       </c>
       <c r="J70" t="n" s="0">
-        <v>199.5279998779297</v>
+        <v>376.7030029296875</v>
       </c>
     </row>
     <row r="71">
@@ -2383,22 +2383,22 @@
         <v>20</v>
       </c>
       <c r="E73" t="n" s="0">
-        <v>997640.0</v>
+        <v>1351990.0</v>
       </c>
       <c r="F73" t="n" s="0">
-        <v>0.0</v>
+        <v>1065000.0</v>
       </c>
       <c r="G73" t="n" s="0">
-        <v>897676.4705135226</v>
+        <v>151414.29498244822</v>
       </c>
       <c r="H73" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="I73" t="n" s="0">
-        <v>99764.00148659945</v>
+        <v>135199.0020146221</v>
       </c>
       <c r="J73" t="n" s="0">
-        <v>199.5279998779297</v>
+        <v>376.7030029296875</v>
       </c>
     </row>
     <row r="74">

</xml_diff>